<commit_message>
Complete Factory Closing Stock
</commit_message>
<xml_diff>
--- a/Code/CoreAPI/API/ExcelUpload/FactoryClosingStock/Factory Closing Stock.xlsx
+++ b/Code/CoreAPI/API/ExcelUpload/FactoryClosingStock/Factory Closing Stock.xlsx
@@ -84,16 +84,13 @@
     <t>Pcs</t>
   </si>
   <si>
-    <t>02-29-2022</t>
+    <t>29-Apr-2022</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="[$-14009]yyyy/mm/dd;@"/>
-  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -126,7 +123,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -410,7 +407,7 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -481,7 +478,7 @@
         <v>100</v>
       </c>
       <c r="I2">
-        <f>(F:F*H:H)</f>
+        <f t="shared" ref="I2:I7" si="0">(F:F*H:H)</f>
         <v>481100</v>
       </c>
     </row>
@@ -511,7 +508,7 @@
         <v>100</v>
       </c>
       <c r="I3">
-        <f>(F:F*H:H)</f>
+        <f t="shared" si="0"/>
         <v>340000</v>
       </c>
     </row>
@@ -541,7 +538,7 @@
         <v>100</v>
       </c>
       <c r="I4">
-        <f>(F:F*H:H)</f>
+        <f t="shared" si="0"/>
         <v>481100</v>
       </c>
     </row>
@@ -571,7 +568,7 @@
         <v>100</v>
       </c>
       <c r="I5">
-        <f>(F:F*H:H)</f>
+        <f t="shared" si="0"/>
         <v>340000</v>
       </c>
     </row>
@@ -601,7 +598,7 @@
         <v>100</v>
       </c>
       <c r="I6">
-        <f>(F:F*H:H)</f>
+        <f t="shared" si="0"/>
         <v>340000</v>
       </c>
     </row>
@@ -631,7 +628,7 @@
         <v>100</v>
       </c>
       <c r="I7">
-        <f>(F:F*H:H)</f>
+        <f t="shared" si="0"/>
         <v>340000</v>
       </c>
     </row>

</xml_diff>